<commit_message>
updated glm and output
</commit_message>
<xml_diff>
--- a/RAnalysis/Output/secondary_gene_list.xlsx
+++ b/RAnalysis/Output/secondary_gene_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2800" windowWidth="37200" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="secondary" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="134">
   <si>
     <t>gene</t>
   </si>
@@ -399,6 +399,36 @@
   </si>
   <si>
     <t>KT934029.1</t>
+  </si>
+  <si>
+    <t>CTGATGTAAACTATAACAGTACAAGAAAGTAGAAAACTAACATAAGGCACCAATCTGATGTACTCATGCAAACTATAACTGGGCAAGAAAGTAGAAAANNNNNNNNNNCGTGCAAACTATAACAGTACAAGAAAGTAGAAAACTAGCATATGGCAACAATCTGATGTACTCATGCAAACTATAACCGTGCAAGAAAGTAGAAAACTTGCATAAAGAAAACCTGCATTAATGTCATCAATTACAGACAGTTGTTAGCTCGTCTAGACAATCTGCATTCTTATAACCAGCCTTGGACCGATGTCAACTGTGAAACAACTAGAAAATGTTTATTAATGCAATCAATTTGAGACACCATTAAGTTATGAAATAACGATAAAATCTGCATTAATATCATCAATCTGAAATTGAAAATATGAAACAGTTAGAAACTGTCCATGAATGAAATCAATCCAAGTCACTGCTATGAGCTATAACATACCTTATACTATTAGAACAACACCAGCTGACTGGTAGTCTAACACATTTACATTTTAACACATTACAGGTCATATATGGCATTCAGATTCATTTTGTAAAGGAATACCTCAGAAAACAACTGAAAAGACCTCACTTCATCCAAACGTAACTGACAACCAACGACTTCAGTGGTGAATGTAAAGTGATCTTGAGACGCCCCCTGATACCACCTTGCCACAACAGAACCCAATGCCAACTGAAGTTTGAGGAAAATATGAATGTACAGCCCATTCACCAATCGCAATACCGTTTTTTTATCAGAATACCTGTAAGGCAAAATTACTGTATACACAGGAAATCTTTTTTCCATGACAGTTAACTTGTTTCTGAAAATATTAACCTTTAAACCGTATAACAGAATCAATTTACAACGCTATTTCTATTTAACTGTAAAAGAACATGGATGCAGCAGACTAACAAAACTGTTACTTTACTCAAACGCCCTAAGGTAGGGCTTCATCCATGGATCCCCACTCTGACTCTTGTGCAGAAGTATACGCAGGCAGTTGTAACTTCTCATCTGCTCCCTCTTTCGTCTGCACTGGAGCAACTGTAGACCCTTACCTGTGAACTGCATCATCAGATCTTTCTTTTCCCTCTCTTCTTTAGCTTTCAACACTCTCTGTCTCTCTAACTCCTCAGCCCTAGCCCATCTCTCTTCCTCTGCCTTCTGCACCGCCATCCTCGCTTTCTTCTCGCGTTCACGTAGCATCCGCCTTACATTCTGTCTGGCTTCCTTCCTTCGTCTGTCAGTTACACACCTGTAGTCTATAACAACTTCTTCCAGAGGACACCAGTTTACGTCTTCTTTTTCAGTCAGACGGAGTCTTTCTAACCGTTTTGCCAATTCATCAATCTCATCCTGAAAAACACTTTTATCATACTTAAAAAACTTTTTATCATTGTTCAAACTCAGTCTACTAAACCTCTGAATGACTGTGTTCAAGTCTTCCTGAAAACCGTCGTCAAGTTCTTGTGTGAATGTTCGTCTGTTGTCAATGTCATGGTCACGGTCAGTGTCAACAGCATACTTACCAGATCTGTAGCGGATAAACGCTTCCGGGACAGATTCAGACACTCCTGAAAACAGAAAATGTTAAAACAGTAATATTAAGACTGAGTGAATGAATGAACGAACAATTTTTGATGTAAATGTATACGATTATTTATTATATAAATAATATTATATTTGATTTTGACCTCCTGAACCAATAAACACATTTTGTATGATTAGGATGTCAAAAGAAACAGCTTGGTTTGGATGTTTTTGTTCTCTTTTGAATTAGAAATTAAATATTTTATAGTTACATTTTGTGATTATATATTTTCGTTCTTTTTAAATCAATAAATAAATCGAATTTTATTTTTAATACTTTTCGGATGACTGTATCACCCGCTGTCTTCGCGCTATATGTACAATGTTAGTCACAGAGGACATAATCATAGATCGTTCATGTTGTGTGTTATAAGTTTGCTGTGCATTATGGTGACCGTTACCTGTGGATGACAAGTATGCCTAATAGTATTATCATTTTTTTAAAATAACAATAATTCTTGAATGCTTGCATTATATATACATGTGTATTTAACAATTAGATAATAACAAGGGTACAATCATATCATAACGAGATATGTTTCATAATTCTTACATACATCGGGCAATTGGAACTGAACTGAAACAATCCCATTTTATTTGGTAAACATTGCATTAAAACAGAGCTATTTAATAACCCAGAATTATGTGGAGCGTCAGGAAGACTTGAGCGTGATTGGTCTAAGTTGTAAGAAAACATCGAACTTAGCCGGTGTTTTGTCATTAGAAACATTGTATTAAAATTTCAAAAGATTTTATTCAAGCATTCATAAGTTATTGCACGGAAACCAAATTGTGACGGACGGACAGACACAAATTAGTGTCTCCCGCTTTTCGCAAACATTGTATATGTATATGTTATGGCTGTTTATATTTATGATAGCAAGACGCATGCACATTTAGCCATAAGACTAATTCTACATCAGTATACAAAGTAGATTCTAATATTGGTAGAACTGGTAGATATGTAGCAAAGAGAAATAAGATAAAAAGTGAGATATGTAAAATAGAATAGAAAGTCACCTTTGATCACTGTGGCGGGTGAATGTTTGCCACGGCGATCAGAGAAGAAAATCTTGAATCTACCACAGGCGCTATAGAAAAAAGAGAGAAAGAACAGTCGTATAACATGTGTATTTAAGGGAAATATTGACGCACATGTCAAGTTATATCATAAAGACAGTGTGTAAGAAATAACCAGGGTGCAGAATTGGGAGGACGACCTTACCATGATCACAATTCCCACCAAACTACCCTCATGGCATCTATATAGACAAGAAATTATTCCAAATTGTGCACAAAATTTGATGTACTCTTCTAGGCCAATTAACTTCATGAAAACTTGATGGTTAAAAAGAGATTTAGTTACTGTTTTTCTCGTTAGACCGCTATACGTATTACTACTGTTAACAGTATCTCCAGCTTGAAGGACTAGTTGCGCCATAGCACACACTGATGAGACGGTGCTGCGCACTTTGACTATACCAGTGACGTTGGGATATTACCCGTACCAGCGACTTACCTGCTAATCGAAAGTACGAGAGTGTTTAGAACACGTATTTATACAAAGAGTGTGGCAATGGCGAAGTCCATTTAAAGTATCAGTGTTTTAATCGAAAAAGTACTTTGCTAGCATTGCCAAAAAAATCAATATATAAAATATATTTAAATAGAGAATAAGTGTTGAATTATAATGTTCAGTGTTAGCGAGTCAATTGAACAGTGACTAAATTACATTTTTATACCGCCCCAATGATGCAAAATGGTACAAGGTGCCTTCTTATTTCATAAACACTTGGTACTTTATTGCACTGTGGGGACGATCGTCCCATTAGAGCAGTAAGGTACTAAGTGCATATGAAATATGAAGGCTTTTGGTACCTTTTTGCTCCAATGGAGCGATTAACATGTCTCTGTTTTGAAACTTATTTTATAACTGAAAAATCATACCTCATAATTTCACTATTTCAAATAGTGAATTTATCAAATATAAATCATTAAAAATCTCGACAGTTCATAACAAACAATAAAAGAGATACGCACAACTTCTTTTTGTGCAAACCACAATTATCGTTAAATAATCATATTCTTGATTAGCAGGTTGGTTGGTCGTCGTGATCTTAACCATAGAAAATGTCTTCATAAAGCACTGAGCGGTCGTCTAGTTTATTGAGATGCTGAGTTTCACATTTCAATGGTAAATAACACGTTTAATTTAAAATAAGAACTATCATTTCATTATTCTATTTTAGGGAAAGTGATTATTTGCTTTTGTACTTACACAAATCCGACAGCAACAAGTATCAACAAAGGCACTATCCTGAAATATACATGTACATTAAAAGTTAAGATCAGTTTGAATATTAATTGTCATTTTTATGCCAGACGATCAGTTCACCTGACCACTCTTTCCTGGGATACAGGAAGGTTAACCAGTACTCGAGCAAACCTATCTCCGCAAGAAACTAATACTAGTAACTTTCGCACTTTCAAAAATCGACGATGAGAGTCGAATGACAATATTAAAGACGCACTGTCGTATGTTTATCATCACAGAGACTGTGGCCGGGCGGGAATTCGGCGTTACAACCCCTGGATTGATAGTCAGATATGCTACCGACTGAGCTAATCGAGCCCGGCTTGAAAGTTAAGAACTTTTTCTTTGATTGATTCAGACAAAATTTCTGAAATCTCGGTCTGTGAGTTTTAAAAAGTCGCTCGGATGTAGTGGAAATATACCTAAATGAGCGGGGCGGTAGTACAAAGAGTGTTATCCACTCACGCCAGGGTTCGCGGGTGAAATCCTAAGTCGCTCTGGTGTAGTGGAAATATACCTGAATGAGCGTGGCGGTAGTACAAAGAGTGTTATCCACTCACGCCAGGGTTCGCGGGTTAAATCCTAAGTCGCTCTGGTGTAGTGGAAATNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNTATCCACTCACGCCAGGGTTCGCGGGTTTAATCCTAAGTCGCTCTGGTGTAGTGGAAATATACCTGAATGAGCGGGGCGGTAATACAAAGAGTGTTATCCACTCACGCCAGGGTTCGCGGGTTAAATCCTAAGTTCAACCAGATGACTTCGCAAAAACAATACTCAGAACTGGTTATATCCAGGAAACGGATTTGTGAACGGTGAATATGCTGCAAGATTATTTGGCACTCGAGCTAACACAATGAGCGATTCCTTCGCTAAAAGTGGGATACCCTCTACCAATACAATATAGACACAGTGGAAGTTAAGAGAAATGTATTTGATGAAAGTATTGTAATAAAGAAAAATAAATAAATTGAATGATTGATTGAATAAATAACACCCATGTAATATTTCTGCATACTTCAAGGGATGAAAATTTAACTTTATTTCAACTTGCGGGTTTGTGGTAGAATTTTCGCCTGGAAATGGGTAATTCGGAGGTTGAAAACATTGTAATGACAACTTCATAGATGTGCCTATGTTTGCATCAGTATACAATGCTCCAGACAGGCTGTGTTATTTTTAATTGATTAGTTTACTCCTTTAATGTGTACAGTATGTATTGATTACTTTCTAATTAAATTTCTATTTAAAATAGCAACGTTGAAATTGTCAGTATTCACTGCTAGTACATGTTGCTTATCAACAAATAAAAACACATTTTTTCTAATTCAATTACCGAACTCCTTTCAGAATTTTTAGTACTTTGATTCAACGTTTAATTTGAGCACCCACTTCTCTCGGACAAAAAGTCCTCCGTGGCCGAGTAGTCTAGGTCGCTGTCTCAAAAAGCATTTACCTGAACTATATCATGAACTGAATGTAAACATGAGTAAAAATATAACTCTTTTGGAATAATAAGATGTAATGACACCTAAAATTTACTGTTTAGTGCACTTATTTCAACCAAAGGTTTTTATATTAAATAGCATATATGGAGTAAAAATATAAACTGCCTATCAACCAGATGAGCAGTTGTTTTAGGGGTAAATAAAATGATCTGTTTTTTTTTTCAAAATCGGCTAAATACTATTATAAATATCACAAAAACAGAAGACTTAAGTGGGCAAAAGTCATTGAAAAAAATATTGGCATATACCTACATAAAAAAATATGAGAGTTTTGAAGGAAAAAAATAAATTTATAGATCTATATGCATATATTAATTTTAAATCTTGATGAATATGTGGTAAATGCAACAATTAAGAAATGCCGAAAGTGTTATCACAAAAAAATCATCAGTTGCTGCAAGCTACTAGTATCCAAACGTTTGACATTTTTTCAACACAAATTTTGCATTGATTTCGCCTATTGAAAAATCAGATTGTGTTGTAAAAATCGTTTTATTCAACAGTAAAACCGCTGATAAATATAAATCTTATTATGTGTATATATGCCACGAAAATTGTATTTATAAATGCTAACAGACGGTTACAAATCCTATTATTCCCCTTGACGGATGCAATTTTCTGTAAATAAATGTCTTAGTGTTGATCCCTACACACCAGGAGCATGTTCTGGGTCCACGGGCATAACACTTTTATTTATCAATATTACTTAACAGAAATATTTTACGTATCATGTTCTATATTGTGTTAGTTCCAGTAGGTTTAACTTGTTTCGCTGCTGGCGTCCACGGGTATAACACTTTTAATTATCAATATTACTTAACGGAAATGTTTTACGTATAATGTTCTATATTGTGTTAGTTCCAGTAGGCTTAATTTGTTTCACTGTTCTAAATTTTGTTAAGTTCCTGTAGGCTCAACTTGTTTCACTGTTCTATATTGTGTTAAGTTCCAGTAGGCTTAACTTGTTTCGTTGTTGGCATTAAATAGATAGTTAAACAAAATACCCCACCCACGCGGACTTTATATGAAACTACAAAAGTACTTAATCTAACATGAAAAATAACACAAAACATTAAATTATTATGACCATTAATTCATTAAAGTATACATACAAGAGTTGGACAAAGTCCAGACGTGCGACGATCTCCGATAATGCCATGTTTTCACTTTTTTGAGAGCGTGTTTTCTTTCAAACGAGAAACAATCAAGCTACAAAATGTAACTAATAGTAACGGCACCGGATGTTGACGTTGCCGGCAGTGCGCGCG</t>
+  </si>
+  <si>
+    <t>MF668234.1</t>
+  </si>
+  <si>
+    <t>TTAGAAAAGCAAGCGTCGCATATAATCAAGACTACATGAGTATCCACTTACTGTGCATACCTCCGTACCACCGCCATAGTACATGCAGTAACGTCCACCATGACCCCCATATCCACCGCCATAGTACATGCAGTAACCTCCACCATGACCTCCGTACAACGGCCATAGTACATGCAGTAACGTCCACCATGACCTCCATATCCACCGCCATAGTAAATGCAGTAACGTCCATCATGACCTCCTTACCACGGCCATAGTACATGCAGTAACGTCCATCATGACCTCCGTACCACGGCCATAGTACATGCAGTAACCTCCACCATGACCTCCATACCACCGCCATAGTACATGCAGTAACCTCCACCATGACCTCCGTACNNNNNNNNNNTCCGTACCACCGCCATATCCCATGCCGTACCATCCACCATAACCTCAGTACCACCGCCATATTCCAT</t>
+  </si>
+  <si>
+    <t>CP020621.1</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>glycine-rich RNA-binding protein 2-like</t>
+  </si>
+  <si>
+    <t>ATGTGTTGGGCGGGGTTCGGTGAAGGCAGCAGGCGGGGATTGGTAAAGGCAGCAGTCGAACTCATTATTTGGGTTGTACGTGTTGGGCTAGGTTTGGTGAAGGCAGCAGGCGGGGTTTGGTAAAGGCAGCAGTAGGGGGTTCGGTAAAGGCAGCAGTCAAACTCATTATTTGGGTTGTACGTGTTGGGCGAGGTTCGGTGAAGGCAACAGGTAGAGATTGGTAAAGGCAGCAGTCGGGGGTTCGGTAAAGGCAGCAGCCGAACTCAATATTTGGGTTGTACGTGTTGGGCGAGGTTCGGTGAAGGCAGCAGGCGGGGTTTGGTAAAGACAGCAGTCGATCTCACTATTTGGGTTGTACGTGTTGGGCGGGGTTCGGTGAAGACAGCAGGCGGGGATAGGTAAAGGCAGCAGTCGAACTCACTATTTGGGTTGTATGTGTTGGGCGGGGTTCGGTAGAGGCAGAAGTCAATCTCACTATTTGGGTTGTACGTGTTGGGCGGGGTTCGGTAGAGGCAGCAGACGGGGTTTGGTAAAGACAGCAGTCGATCTCACTATTTGGGTGTGTTGGGCGGGGTTCCGTAGAGGCAGTAGTCGATCTCACTATTTGGGTTGTATGTGTTGGGCGGGGTTCGGTGAAGGCAACCGGCTGGGTTCGGTAGAGGCAGTAGTCGATCTCACTATTTGGGATGTACGTGTTGGGCGGGATTCGGTAGAGGCAGTAGTCGATCTCACTATTTGGGTTGTACGTGTTGGGCGTGGTTCGGTAGAGGCAGTAGCCGATCTCACTATTTGGGTTGTACGTGTTGGTCGGGGTTCGGTGAAGGCAACAGGCGGGGTTCGGTAG</t>
+  </si>
+  <si>
+    <t>rho GTPase-activating protein 15-like</t>
+  </si>
+  <si>
+    <t>XM_022380211.1</t>
+  </si>
+  <si>
+    <t>ATGTCGCCAATTTTCCTCCTACCCCAACCAATTCCTCTTGTTCCAACACGACTACATCAACAATACATGACAAACATATCGCCAATTTCCACCTAACCAACCATTTCTTCTCTTCTTGTCCCAACACGCCTATATCACCAATACATAACAAACATATCGTCAATCTCAACTTACCCAACCATATTTTCTTGTTCCACCACCACAACATCAATCACCAAGACATGACAAATATAATCGTCAATATCCACCTACTCCAACCATTTCGACTTGTTCCAACACGACTACATCGCCAATACATGACAAATATATCGCCAATGTCCACCTACCCGAACCATGTCCTCTTGTTCCAACACGACTACATCACCAATGCATGACAAATATATATCGACAATTTCCACATACCGAAACAATTTCGTATTGTTCCAACACACAAACGTCACCAATACATGACAAACATAATCGCCAATTTCCACCTACCCCATCCATTTCCTCTTGTTCCACAACGACTACATCACCAATACATGACAAATATATTGCCAATTTCCAACTACCCNNNNNNNNNNAATATATCGCCAATTTCCAACTACCCAACCATTTCCTCTTGTTCCACTACGACTACATCACCAATACATGACAAATATATCGCAAATTTCCACAAACACATGTGAAGACTTGTGTAATGTTTCAATCAAATACATTGAGTGGTTGGTGAGATATGGAGTTGATGGTACTTGCACGCTTAATTTTAACCAGAATTTTAAAGTCAAACAAGGGCAAAATTTGTATTATATTCATACAAAAGTTATCTAA</t>
   </si>
 </sst>
 </file>
@@ -409,7 +439,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -420,6 +450,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -448,9 +486,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -459,8 +498,9 @@
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -736,10 +776,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W101"/>
+  <dimension ref="A1:X101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,10 +791,10 @@
     <col min="9" max="9" width="17.6640625" customWidth="1"/>
     <col min="15" max="15" width="17.33203125" customWidth="1"/>
     <col min="20" max="21" width="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16" customWidth="1"/>
+    <col min="22" max="23" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -816,10 +859,13 @@
         <v>122</v>
       </c>
       <c r="W1" t="s">
+        <v>128</v>
+      </c>
+      <c r="X1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>115</v>
       </c>
@@ -883,11 +929,12 @@
       <c r="V2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="4"/>
+      <c r="X2" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>75</v>
       </c>
@@ -942,8 +989,20 @@
       <c r="R3" s="3">
         <v>8.5174572755942702E-6</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T3" s="2">
+        <v>20247275</v>
+      </c>
+      <c r="U3" s="2">
+        <v>20254070</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -998,8 +1057,23 @@
       <c r="R4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T4" s="2">
+        <v>18663212</v>
+      </c>
+      <c r="U4" s="2">
+        <v>18663666</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -1054,8 +1128,17 @@
       <c r="R5" s="2">
         <v>0.54504663429446798</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T5" s="2">
+        <v>25439847</v>
+      </c>
+      <c r="U5" s="2">
+        <v>25479614</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>52</v>
       </c>
@@ -1110,8 +1193,23 @@
       <c r="R6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T6" s="2">
+        <v>9064986</v>
+      </c>
+      <c r="U6" s="2">
+        <v>9065829</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>61</v>
       </c>
@@ -1166,8 +1264,17 @@
       <c r="R7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T7" s="2">
+        <v>25509336</v>
+      </c>
+      <c r="U7" s="2">
+        <v>25510145</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>105</v>
       </c>
@@ -1223,7 +1330,7 @@
         <v>1.3251194601030299E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>78</v>
       </c>
@@ -1279,7 +1386,7 @@
         <v>2.73043191430496E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>91</v>
       </c>
@@ -1335,7 +1442,7 @@
         <v>1.2235368328344401E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
@@ -1391,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
@@ -1447,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -1503,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>87</v>
       </c>
@@ -1559,7 +1666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1615,7 +1722,7 @@
         <v>9.86731108340168E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>69</v>
       </c>
@@ -6436,5 +6543,6 @@
     <sortCondition ref="O2:O101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>